<commit_message>
Alterações para orientação a objeto
</commit_message>
<xml_diff>
--- a/teste.xlsx
+++ b/teste.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <si>
+    <t>Brasal Empreendimento</t>
+  </si>
   <si>
     <t>teste11</t>
   </si>
@@ -25,6 +28,9 @@
     <t>teste31</t>
   </si>
   <si>
+    <t>Azship tecnologia</t>
+  </si>
+  <si>
     <t>teste12</t>
   </si>
   <si>
@@ -32,6 +38,12 @@
   </si>
   <si>
     <t>teste32</t>
+  </si>
+  <si>
+    <t>expresso nacional</t>
+  </si>
+  <si>
+    <t>Bem Brasil</t>
   </si>
   <si>
     <t>teste13</t>
@@ -92,12 +104,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -405,58 +426,66 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="40.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="40.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
-      <c r="A1" s="1">
-        <v>15405030000155</v>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="1">
-        <v>22894852000102</v>
+      <c r="A2" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="1">
-        <v>27035444000119</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="3" t="s">
         <v>8</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correção do retorno da função que lista os dados das empresas
</commit_message>
<xml_diff>
--- a/teste.xlsx
+++ b/teste.xlsx
@@ -83,7 +83,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -100,25 +100,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -432,23 +430,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="40.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="40.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -456,35 +454,35 @@
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adicionado o retorno das informações para a planilha, limpeza de codigo
</commit_message>
<xml_diff>
--- a/teste.xlsx
+++ b/teste.xlsx
@@ -14,45 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="3">
   <si>
-    <t>Brasal Empreendimento</t>
+    <t>Grupo Serquímica</t>
   </si>
   <si>
-    <t>teste11</t>
+    <t/>
   </si>
   <si>
-    <t>teste21</t>
-  </si>
-  <si>
-    <t>teste31</t>
-  </si>
-  <si>
-    <t>Azship tecnologia</t>
-  </si>
-  <si>
-    <t>teste12</t>
-  </si>
-  <si>
-    <t>teste22</t>
-  </si>
-  <si>
-    <t>teste32</t>
-  </si>
-  <si>
-    <t>expresso nacional</t>
-  </si>
-  <si>
-    <t>Bem Brasil</t>
-  </si>
-  <si>
-    <t>teste13</t>
-  </si>
-  <si>
-    <t>teste23</t>
-  </si>
-  <si>
-    <t>teste33</t>
+    <t>azship tecnologia</t>
   </si>
 </sst>
 </file>
@@ -111,16 +81,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -424,67 +409,111 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="40.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="7" width="40.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="19.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="40.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="A3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="A4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Limitando as entradas para 20 empresas
</commit_message>
<xml_diff>
--- a/teste.xlsx
+++ b/teste.xlsx
@@ -14,15 +14,81 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+  <si>
+    <t>BRASAL REFRIGERANTES</t>
+  </si>
+  <si>
+    <t>Mc Bauchemie</t>
+  </si>
   <si>
     <t>Grupo Serquímica</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>azship tecnologia</t>
+    <t>Sementes Cosmorama</t>
+  </si>
+  <si>
+    <t>Cereal Indústria</t>
+  </si>
+  <si>
+    <t>Grupo Cereal</t>
+  </si>
+  <si>
+    <t>Vitral Vidros Planos</t>
+  </si>
+  <si>
+    <t>Rancho King Sementes</t>
+  </si>
+  <si>
+    <t>Porto a Porto</t>
+  </si>
+  <si>
+    <t>Uniggel Sementes</t>
+  </si>
+  <si>
+    <t>Fiasul</t>
+  </si>
+  <si>
+    <t>Fazenda Tradição</t>
+  </si>
+  <si>
+    <t>Cepalgo</t>
+  </si>
+  <si>
+    <t>COMING INDÚSTRIA E COMÉRCIO DE COUROS</t>
+  </si>
+  <si>
+    <t>ESAF CLARIS</t>
+  </si>
+  <si>
+    <t>Comtrafo</t>
+  </si>
+  <si>
+    <t>Elinox</t>
+  </si>
+  <si>
+    <t>Korin Agricultura</t>
+  </si>
+  <si>
+    <t>Korin Alimentos</t>
+  </si>
+  <si>
+    <t>CAW</t>
+  </si>
+  <si>
+    <t>Tecelagem Roma Ltda</t>
+  </si>
+  <si>
+    <t>CooperAgudo</t>
+  </si>
+  <si>
+    <t>Quinta do Vale Alimentos</t>
+  </si>
+  <si>
+    <t>Grupo Adal</t>
+  </si>
+  <si>
+    <t>Specialmix</t>
   </si>
 </sst>
 </file>
@@ -30,13 +96,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -62,16 +134,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
+      <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -81,24 +153,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -409,111 +475,425 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="7" width="40.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="19.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="40.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="40.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="19.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="40.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
+      <c r="A4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+      <c r="A15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+      <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+      <c r="A17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+      <c r="A18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+      <c r="A19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+      <c r="A20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+      <c r="A21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+      <c r="A22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+      <c r="A23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+      <c r="A24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+      <c r="A25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>